<commit_message>
- Première passe dans les fichiers pour mettre les bon numéros d'ids de paroisse. - Au passage suppression de quelques lignes des groupes ostensiblement bidons (ids pas possibles) - Au passage suppression de lignes vides dans certains fichiers.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@20540 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Région 2/2000/supergroup.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Région 2/2000/supergroup.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>_Id</t>
   </si>
@@ -218,12 +218,6 @@
   </si>
   <si>
     <t>DONS</t>
-  </si>
-  <si>
-    <t>ACTIVITES NON CLASSEES</t>
-  </si>
-  <si>
-    <t>__Trv ::Des1</t>
   </si>
 </sst>
 </file>
@@ -584,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -606,7 +600,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="2">
-        <v>4000000000</v>
+        <v>2000000000</v>
       </c>
       <c r="C2" s="3">
         <v>2000000878</v>
@@ -616,8 +610,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="2">
-        <v>4000000000</v>
+      <c r="B3" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C3" s="3">
         <v>2000000879</v>
@@ -627,8 +621,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="2">
-        <v>4000000000</v>
+      <c r="B4" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C4" s="3">
         <v>2000000880</v>
@@ -638,8 +632,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="2">
-        <v>4000000000</v>
+      <c r="B5" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C5" s="3">
         <v>2000000881</v>
@@ -649,8 +643,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="2">
-        <v>4000000000</v>
+      <c r="B6" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C6" s="3">
         <v>2000000882</v>
@@ -660,8 +654,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="2">
-        <v>4000000000</v>
+      <c r="B7" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C7" s="3">
         <v>2000000883</v>
@@ -671,8 +665,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="2">
-        <v>4000000000</v>
+      <c r="B8" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C8" s="3">
         <v>2000000887</v>
@@ -682,8 +676,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="2">
-        <v>4000000000</v>
+      <c r="B9" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C9" s="3">
         <v>2000000888</v>
@@ -693,8 +687,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="2">
-        <v>4000000000</v>
+      <c r="B10" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C10" s="3">
         <v>2000000894</v>
@@ -704,8 +698,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="2">
-        <v>4000000000</v>
+      <c r="B11" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C11" s="3">
         <v>2000000900</v>
@@ -715,8 +709,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="2">
-        <v>4000000000</v>
+      <c r="B12" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C12" s="3">
         <v>2000000925</v>
@@ -726,8 +720,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="2">
-        <v>4000000000</v>
+      <c r="B13" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C13" s="3">
         <v>2000000975</v>
@@ -737,8 +731,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="2">
-        <v>4000000000</v>
+      <c r="B14" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C14" s="3">
         <v>2000001106</v>
@@ -748,8 +742,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="2">
-        <v>4000000000</v>
+      <c r="B15" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C15" s="3">
         <v>2000001145</v>
@@ -759,8 +753,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="2">
-        <v>4000000000</v>
+      <c r="B16" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C16" s="3">
         <v>2000001146</v>
@@ -770,8 +764,8 @@
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="2">
-        <v>4000000000</v>
+      <c r="B17" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C17" s="3">
         <v>2000001149</v>
@@ -781,8 +775,8 @@
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="2">
-        <v>4000000000</v>
+      <c r="B18" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C18" s="3">
         <v>2000001150</v>
@@ -792,8 +786,8 @@
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="2">
-        <v>4000000000</v>
+      <c r="B19" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C19" s="3">
         <v>2000001152</v>
@@ -803,8 +797,8 @@
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="2">
-        <v>4000000000</v>
+      <c r="B20" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C20" s="3">
         <v>2000001157</v>
@@ -814,8 +808,8 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="2">
-        <v>4000000000</v>
+      <c r="B21" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C21" s="3">
         <v>2000001159</v>
@@ -825,8 +819,8 @@
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="2">
-        <v>4000000000</v>
+      <c r="B22" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C22" s="3">
         <v>2000001160</v>
@@ -836,8 +830,8 @@
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="2">
-        <v>4000000000</v>
+      <c r="B23" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C23" s="3">
         <v>2000001161</v>
@@ -847,8 +841,8 @@
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="2">
-        <v>4000000000</v>
+      <c r="B24" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C24" s="3">
         <v>2000001162</v>
@@ -858,8 +852,8 @@
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="2">
-        <v>4000000000</v>
+      <c r="B25" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C25" s="3">
         <v>2000001163</v>
@@ -869,8 +863,8 @@
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="2">
-        <v>4000000000</v>
+      <c r="B26" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C26" s="3">
         <v>2000001164</v>
@@ -880,8 +874,8 @@
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="2">
-        <v>4000000000</v>
+      <c r="B27" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C27" s="3">
         <v>2000001165</v>
@@ -891,8 +885,8 @@
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="2">
-        <v>4000000000</v>
+      <c r="B28" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C28" s="3">
         <v>2000001166</v>
@@ -902,8 +896,8 @@
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="2">
-        <v>4000000000</v>
+      <c r="B29" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C29" s="3">
         <v>2000001167</v>
@@ -913,8 +907,8 @@
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="2">
-        <v>4000000000</v>
+      <c r="B30" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C30" s="3">
         <v>2000001171</v>
@@ -924,8 +918,8 @@
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="2">
-        <v>4000000000</v>
+      <c r="B31" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C31" s="3">
         <v>2000001173</v>
@@ -935,8 +929,8 @@
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="2">
-        <v>4000000000</v>
+      <c r="B32" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C32" s="3">
         <v>2000001174</v>
@@ -946,8 +940,8 @@
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="2">
-        <v>4000000000</v>
+      <c r="B33" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C33" s="3">
         <v>2000001176</v>
@@ -957,8 +951,8 @@
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="2">
-        <v>4000000000</v>
+      <c r="B34" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C34" s="3">
         <v>2000001177</v>
@@ -968,8 +962,8 @@
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="2">
-        <v>4000000000</v>
+      <c r="B35" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C35" s="3">
         <v>2000001178</v>
@@ -979,8 +973,8 @@
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="2">
-        <v>4000000000</v>
+      <c r="B36" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C36" s="3">
         <v>2000001179</v>
@@ -990,8 +984,8 @@
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="2">
-        <v>4000000000</v>
+      <c r="B37" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C37" s="3">
         <v>2000001180</v>
@@ -1001,8 +995,8 @@
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="2">
-        <v>4000000000</v>
+      <c r="B38" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C38" s="3">
         <v>2000001181</v>
@@ -1012,8 +1006,8 @@
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="2">
-        <v>4000000000</v>
+      <c r="B39" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C39" s="3">
         <v>2000001182</v>
@@ -1023,8 +1017,8 @@
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="2">
-        <v>4000000000</v>
+      <c r="B40" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C40" s="3">
         <v>2000001183</v>
@@ -1034,8 +1028,8 @@
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="2">
-        <v>4000000000</v>
+      <c r="B41" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C41" s="3">
         <v>2000001186</v>
@@ -1045,8 +1039,8 @@
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="2">
-        <v>4000000000</v>
+      <c r="B42" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C42" s="3">
         <v>2000001187</v>
@@ -1056,8 +1050,8 @@
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="2">
-        <v>4000000000</v>
+      <c r="B43" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C43" s="3">
         <v>2000001188</v>
@@ -1067,8 +1061,8 @@
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="2">
-        <v>4000000000</v>
+      <c r="B44" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C44" s="3">
         <v>2000001189</v>
@@ -1078,8 +1072,8 @@
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="2">
-        <v>4000000000</v>
+      <c r="B45" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C45" s="3">
         <v>2000001190</v>
@@ -1089,8 +1083,8 @@
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B46" s="2">
-        <v>4000000000</v>
+      <c r="B46" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C46" s="3">
         <v>2000001191</v>
@@ -1100,8 +1094,8 @@
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B47" s="2">
-        <v>4000000000</v>
+      <c r="B47" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C47" s="3">
         <v>2000001192</v>
@@ -1111,8 +1105,8 @@
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="2">
-        <v>4000000000</v>
+      <c r="B48" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C48" s="3">
         <v>2000001193</v>
@@ -1122,8 +1116,8 @@
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="2">
-        <v>4000000000</v>
+      <c r="B49" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C49" s="3">
         <v>2000001194</v>
@@ -1133,8 +1127,8 @@
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B50" s="2">
-        <v>4000000000</v>
+      <c r="B50" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C50" s="3">
         <v>2000001195</v>
@@ -1144,8 +1138,8 @@
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B51" s="2">
-        <v>4000000000</v>
+      <c r="B51" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C51" s="3">
         <v>2000001196</v>
@@ -1155,8 +1149,8 @@
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B52" s="2">
-        <v>4000000000</v>
+      <c r="B52" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C52" s="3">
         <v>2000001197</v>
@@ -1166,8 +1160,8 @@
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B53" s="2">
-        <v>4000000000</v>
+      <c r="B53" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C53" s="3">
         <v>2000001198</v>
@@ -1177,8 +1171,8 @@
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B54" s="2">
-        <v>4000000000</v>
+      <c r="B54" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C54" s="3">
         <v>2000001199</v>
@@ -1188,8 +1182,8 @@
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B55" s="2">
-        <v>4000000000</v>
+      <c r="B55" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C55" s="3">
         <v>2000001200</v>
@@ -1199,8 +1193,8 @@
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B56" s="2">
-        <v>4000000000</v>
+      <c r="B56" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C56" s="3">
         <v>2000001201</v>
@@ -1210,8 +1204,8 @@
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B57" s="2">
-        <v>4000000000</v>
+      <c r="B57" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C57" s="3">
         <v>2000001202</v>
@@ -1221,8 +1215,8 @@
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B58" s="2">
-        <v>4000000000</v>
+      <c r="B58" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C58" s="3">
         <v>2000001203</v>
@@ -1232,8 +1226,8 @@
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B59" s="2">
-        <v>4000000000</v>
+      <c r="B59" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C59" s="3">
         <v>2000001204</v>
@@ -1243,8 +1237,8 @@
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B60" s="2">
-        <v>4000000000</v>
+      <c r="B60" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C60" s="3">
         <v>2000001205</v>
@@ -1254,8 +1248,8 @@
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B61" s="2">
-        <v>4000000000</v>
+      <c r="B61" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C61" s="3">
         <v>2000001206</v>
@@ -1265,8 +1259,8 @@
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B62" s="2">
-        <v>4000000000</v>
+      <c r="B62" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C62" s="3">
         <v>2000001207</v>
@@ -1276,8 +1270,8 @@
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B63" s="2">
-        <v>4000000000</v>
+      <c r="B63" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C63" s="3">
         <v>2000001209</v>
@@ -1287,8 +1281,8 @@
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B64" s="2">
-        <v>4000000000</v>
+      <c r="B64" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C64" s="3">
         <v>2000001210</v>
@@ -1298,8 +1292,8 @@
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B65" s="2">
-        <v>4000000000</v>
+      <c r="B65" s="3">
+        <v>2000000000</v>
       </c>
       <c r="C65" s="3">
         <v>2000001211</v>
@@ -1309,26 +1303,14 @@
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B66" s="2">
-        <v>4000000000</v>
-      </c>
-      <c r="C66" s="3">
-        <v>100000000558</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="4"/>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B67" s="2">
-        <v>4000000000</v>
-      </c>
-      <c r="C67" s="3">
-        <v>0</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Nouvelles version de fichier de la région 02.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@20618 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Région 2/2000/supergroup.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Région 2/2000/supergroup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="555" windowWidth="27495" windowHeight="11445"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="23655" windowHeight="11445"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>_Id</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>DONS</t>
+  </si>
+  <si>
+    <t>ACTIVITES NON CLASSEES</t>
   </si>
 </sst>
 </file>
@@ -576,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -603,714 +606,715 @@
         <v>2000000000</v>
       </c>
       <c r="C2" s="3">
-        <v>2000000878</v>
+        <v>305020100</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>2000000000</v>
       </c>
       <c r="C3" s="3">
-        <v>2000000879</v>
+        <v>305020200</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>2000000000</v>
       </c>
       <c r="C4" s="3">
-        <v>2000000880</v>
+        <v>305020300</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>2000000000</v>
       </c>
       <c r="C5" s="3">
-        <v>2000000881</v>
+        <v>305020400</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>2000000000</v>
       </c>
       <c r="C6" s="3">
-        <v>2000000882</v>
+        <v>305020500</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>2000000000</v>
       </c>
       <c r="C7" s="3">
-        <v>2000000883</v>
+        <v>305020600</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>2000000000</v>
       </c>
       <c r="C8" s="3">
-        <v>2000000887</v>
+        <v>305020700</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>2000000000</v>
       </c>
       <c r="C9" s="3">
-        <v>2000000888</v>
+        <v>305020800</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>2000000000</v>
       </c>
       <c r="C10" s="3">
-        <v>2000000894</v>
+        <v>305020900</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>2000000000</v>
       </c>
       <c r="C11" s="3">
-        <v>2000000900</v>
+        <v>305021000</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>2000000000</v>
       </c>
       <c r="C12" s="3">
-        <v>2000000925</v>
+        <v>305021100</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>2000000000</v>
       </c>
       <c r="C13" s="3">
-        <v>2000000975</v>
+        <v>305021200</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>2000000000</v>
       </c>
       <c r="C14" s="3">
-        <v>2000001106</v>
+        <v>305021300</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>2000000000</v>
       </c>
       <c r="C15" s="3">
-        <v>2000001145</v>
+        <v>305021400</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>2000000000</v>
       </c>
       <c r="C16" s="3">
-        <v>2000001146</v>
+        <v>305021500</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>2000000000</v>
       </c>
       <c r="C17" s="3">
-        <v>2000001149</v>
+        <v>305021600</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>2000000000</v>
       </c>
       <c r="C18" s="3">
-        <v>2000001150</v>
+        <v>305021700</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>2000000000</v>
       </c>
       <c r="C19" s="3">
-        <v>2000001152</v>
+        <v>305021800</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>2000000000</v>
       </c>
       <c r="C20" s="3">
-        <v>2000001157</v>
+        <v>305021900</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>2000000000</v>
       </c>
       <c r="C21" s="3">
-        <v>2000001159</v>
+        <v>305022000</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>2000000000</v>
       </c>
       <c r="C22" s="3">
-        <v>2000001160</v>
+        <v>305022100</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>2000000000</v>
       </c>
       <c r="C23" s="3">
-        <v>2000001161</v>
+        <v>305022200</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>2000000000</v>
       </c>
       <c r="C24" s="3">
-        <v>2000001162</v>
+        <v>305022300</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>2000000000</v>
       </c>
       <c r="C25" s="3">
-        <v>2000001163</v>
+        <v>305022400</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>2000000000</v>
       </c>
       <c r="C26" s="3">
-        <v>2000001164</v>
+        <v>305022500</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>2000000000</v>
       </c>
       <c r="C27" s="3">
-        <v>2000001165</v>
+        <v>305022600</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>2000000000</v>
       </c>
       <c r="C28" s="3">
-        <v>2000001166</v>
+        <v>305022700</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>2000000000</v>
       </c>
       <c r="C29" s="3">
-        <v>2000001167</v>
+        <v>305022800</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>2000000000</v>
       </c>
       <c r="C30" s="3">
-        <v>2000001171</v>
+        <v>305022900</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>2000000000</v>
       </c>
       <c r="C31" s="3">
-        <v>2000001173</v>
+        <v>305023000</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>2000000000</v>
       </c>
       <c r="C32" s="3">
-        <v>2000001174</v>
+        <v>305023100</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>2000000000</v>
       </c>
       <c r="C33" s="3">
-        <v>2000001176</v>
+        <v>305023200</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>2000000000</v>
       </c>
       <c r="C34" s="3">
-        <v>2000001177</v>
+        <v>305023300</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>2000000000</v>
       </c>
       <c r="C35" s="3">
-        <v>2000001178</v>
+        <v>305023400</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>2000000000</v>
       </c>
       <c r="C36" s="3">
-        <v>2000001179</v>
+        <v>305023500</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>2000000000</v>
       </c>
       <c r="C37" s="3">
-        <v>2000001180</v>
+        <v>305023600</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>2000000000</v>
       </c>
       <c r="C38" s="3">
-        <v>2000001181</v>
+        <v>305023700</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="3">
+      <c r="B39" s="2">
         <v>2000000000</v>
       </c>
       <c r="C39" s="3">
-        <v>2000001182</v>
+        <v>305023800</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="3">
+      <c r="B40" s="2">
         <v>2000000000</v>
       </c>
       <c r="C40" s="3">
-        <v>2000001183</v>
+        <v>305023900</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <v>2000000000</v>
       </c>
       <c r="C41" s="3">
-        <v>2000001186</v>
+        <v>305024000</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <v>2000000000</v>
       </c>
       <c r="C42" s="3">
-        <v>2000001187</v>
+        <v>305024100</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <v>2000000000</v>
       </c>
       <c r="C43" s="3">
-        <v>2000001188</v>
+        <v>305024200</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="3">
+      <c r="B44" s="2">
         <v>2000000000</v>
       </c>
       <c r="C44" s="3">
-        <v>2000001189</v>
+        <v>305024300</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <v>2000000000</v>
       </c>
       <c r="C45" s="3">
-        <v>2000001190</v>
+        <v>305024400</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B46" s="3">
+      <c r="B46" s="2">
         <v>2000000000</v>
       </c>
       <c r="C46" s="3">
-        <v>2000001191</v>
+        <v>305024500</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>2000000000</v>
       </c>
       <c r="C47" s="3">
-        <v>2000001192</v>
+        <v>305024600</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="3">
+      <c r="B48" s="2">
         <v>2000000000</v>
       </c>
       <c r="C48" s="3">
-        <v>2000001193</v>
+        <v>305024700</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <v>2000000000</v>
       </c>
       <c r="C49" s="3">
-        <v>2000001194</v>
+        <v>305024800</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>2000000000</v>
       </c>
       <c r="C50" s="3">
-        <v>2000001195</v>
+        <v>305024900</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B51" s="3">
+      <c r="B51" s="2">
         <v>2000000000</v>
       </c>
       <c r="C51" s="3">
-        <v>2000001196</v>
+        <v>305025000</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B52" s="3">
+      <c r="B52" s="2">
         <v>2000000000</v>
       </c>
       <c r="C52" s="3">
-        <v>2000001197</v>
+        <v>305025100</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B53" s="3">
+      <c r="B53" s="2">
         <v>2000000000</v>
       </c>
       <c r="C53" s="3">
-        <v>2000001198</v>
+        <v>305025200</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B54" s="3">
+      <c r="B54" s="2">
         <v>2000000000</v>
       </c>
       <c r="C54" s="3">
-        <v>2000001199</v>
+        <v>305025300</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B55" s="3">
+      <c r="B55" s="2">
         <v>2000000000</v>
       </c>
       <c r="C55" s="3">
-        <v>2000001200</v>
+        <v>305025400</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B56" s="3">
+      <c r="B56" s="2">
         <v>2000000000</v>
       </c>
       <c r="C56" s="3">
-        <v>2000001201</v>
+        <v>305025500</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B57" s="3">
+      <c r="B57" s="2">
         <v>2000000000</v>
       </c>
       <c r="C57" s="3">
-        <v>2000001202</v>
+        <v>305025600</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B58" s="3">
+      <c r="B58" s="2">
         <v>2000000000</v>
       </c>
       <c r="C58" s="3">
-        <v>2000001203</v>
+        <v>305025700</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B59" s="3">
+      <c r="B59" s="2">
         <v>2000000000</v>
       </c>
       <c r="C59" s="3">
-        <v>2000001204</v>
+        <v>305025800</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B60" s="3">
+      <c r="B60" s="2">
         <v>2000000000</v>
       </c>
       <c r="C60" s="3">
-        <v>2000001205</v>
+        <v>305025900</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B61" s="3">
+      <c r="B61" s="2">
         <v>2000000000</v>
       </c>
       <c r="C61" s="3">
-        <v>2000001206</v>
+        <v>305026000</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B62" s="3">
+      <c r="B62" s="2">
         <v>2000000000</v>
       </c>
       <c r="C62" s="3">
-        <v>2000001207</v>
+        <v>305026100</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B63" s="3">
+      <c r="B63" s="2">
         <v>2000000000</v>
       </c>
       <c r="C63" s="3">
-        <v>2000001209</v>
+        <v>305026200</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B64" s="3">
+      <c r="B64" s="2">
         <v>2000000000</v>
       </c>
       <c r="C64" s="3">
-        <v>2000001210</v>
+        <v>305026300</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B65" s="3">
+      <c r="B65" s="2">
         <v>2000000000</v>
       </c>
       <c r="C65" s="3">
-        <v>2000001211</v>
+        <v>305026400</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="4"/>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="4"/>
+      <c r="B66" s="2">
+        <v>2000000000</v>
+      </c>
+      <c r="C66" s="3">
+        <v>305026500</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>